<commit_message>
Update test file and data used
</commit_message>
<xml_diff>
--- a/expressways/core/tests/data/Test_Proforma.xlsx
+++ b/expressways/core/tests/data/Test_Proforma.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UKMXA046\Development\dev-tools\Projects\expressways\expressways\core\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4DF79F-B1BE-4C20-8FBF-A7AD3324B701}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290284E4-47FC-405B-BEBB-F8E22D1279AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="394" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="394" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Sheet" sheetId="5" r:id="rId1"/>
+    <sheet name="Invalid Sheet" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -90,8 +91,68 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Canaway, Ian</author>
+    <author>Gregory, Rob</author>
+  </authors>
+  <commentList>
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{781545B6-C421-4BA4-B275-F2FF08D4FD72}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Canaway, Ian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2.39 - years from which dataset covers. Divide by 2.39 to give per mile basis.
+115 - 2 way distance of the routes from which dataset covers. i.e. divide by 115 to get per mile basis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="1" shapeId="0" xr:uid="{DF8DE4F3-7BEB-4E0F-9B5E-F7E0E4CAFDBF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gregory, Rob:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Updated frequency with mis-reporting added and % difference from Stats19</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="41">
   <si>
     <t>Yes</t>
   </si>
@@ -794,7 +855,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -901,6 +962,9 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -925,6 +989,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -934,6 +1004,27 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -943,46 +1034,19 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1271,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAF14C7-8305-4FE8-8798-9C94FB1D6030}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -1289,106 +1353,106 @@
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
-      <c r="P2" s="44" t="s">
+      <c r="P2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="44" t="s">
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="44" t="s">
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="44" t="s">
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="46"/>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="49"/>
     </row>
     <row r="3" spans="1:31" s="11" customFormat="1" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="53" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="54"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="56"/>
       <c r="O3" s="35"/>
-      <c r="P3" s="47" t="s">
+      <c r="P3" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="49"/>
-      <c r="T3" s="50" t="s">
+      <c r="S3" s="59"/>
+      <c r="T3" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51" t="s">
+      <c r="U3" s="46"/>
+      <c r="V3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="W3" s="52"/>
-      <c r="X3" s="62" t="s">
+      <c r="W3" s="60"/>
+      <c r="X3" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="48" t="s">
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="60" t="s">
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="51" t="s">
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="AE3" s="52"/>
+      <c r="AE3" s="60"/>
     </row>
     <row r="4" spans="1:31" s="11" customFormat="1" ht="56.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="59"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="7" t="s">
         <v>20</v>
       </c>
@@ -1656,11 +1720,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="L3:N3"/>
@@ -1671,55 +1730,365 @@
     <mergeCell ref="T2:W2"/>
     <mergeCell ref="X2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K6" xr:uid="{CE310003-786F-40A4-917F-0B93ED1CA802}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M6 G5:J6" xr:uid="{553B034D-559B-409D-B756-2F31D4AB2AA4}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE310003-786F-40A4-917F-0B93ED1CA802}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>K5:K6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{553B034D-559B-409D-B756-2F31D4AB2AA4}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>I5:I6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{06BCB54D-1008-44DC-92B0-DBF127E51FDA}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H5:H6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CF016AD1-149B-439D-9DA5-4C2DD8F17E00}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>M5:M6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{84ABF24D-F3E8-4ABB-B03D-FA843B803A7A}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J5:J6 G5:G6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E603F408-1480-4F67-B567-3382CF3835BE}">
+  <dimension ref="A1:AE5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:31" s="11" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:31" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="49"/>
+    </row>
+    <row r="3" spans="1:31" s="11" customFormat="1" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="55"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="59"/>
+      <c r="T3" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" s="60"/>
+      <c r="X3" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" s="60"/>
+    </row>
+    <row r="4" spans="1:31" s="11" customFormat="1" ht="56.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="U4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" s="33" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="26">
+        <f>($N5/2.39)/115</f>
+        <v>5.0936874658904854E-2</v>
+      </c>
+      <c r="M5" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="N5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="29">
+        <v>0</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="29">
+        <v>0</v>
+      </c>
+      <c r="U5" s="29">
+        <v>0</v>
+      </c>
+      <c r="V5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" s="29">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA5" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE5" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5 G5:J5" xr:uid="{879B92CC-322A-4578-8FFF-AD310552F718}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5" xr:uid="{6C635E90-4790-4257-95F5-A614D805CF38}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDD8288D38F1C42A36FEDCC78DC6D6E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="89580e21d3f96c966d8f06eb05e6172d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7bfdba5a-f2ca-49df-8aab-4bf22a4d1721" xmlns:ns3="919975a2-1b12-4f17-b770-554a166c605d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6d01a5ea674bc351d086591d07de591" ns2:_="" ns3:_="">
     <xsd:import namespace="7bfdba5a-f2ca-49df-8aab-4bf22a4d1721"/>
@@ -1922,22 +2291,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4130628F-86D4-4759-9ED7-A11EA337C3EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708582EC-5084-4A9B-BDF1-D166F4F7F696}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1956,19 +2324,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{892B8B7D-89AB-4374-80BA-70C591A11EAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4130628F-86D4-4759-9ED7-A11EA337C3EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>